<commit_message>
Adding LTE001 and WHS001test data
</commit_message>
<xml_diff>
--- a/TestData/OPR293_DeliveryDocumentation_TestData.xlsx
+++ b/TestData/OPR293_DeliveryDocumentation_TestData.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v-ssaha1\Desktop\ICargo KT\Test data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v-vkaushal\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F51405B0-7EEE-4D53-9A49-45EE97EF2883}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24FE70D5-EA58-4646-BAF7-8133354B422C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="3" xr2:uid="{7916E571-AC3D-4576-B5B7-2150EE7F4F02}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="22920" windowHeight="13815" activeTab="3" xr2:uid="{7916E571-AC3D-4576-B5B7-2150EE7F4F02}"/>
   </bookViews>
   <sheets>
     <sheet name="OPR293_DLV_00001" sheetId="1" r:id="rId1"/>
     <sheet name="OPR293_DLV_00004" sheetId="2" r:id="rId2"/>
     <sheet name="OPR293_DLV_00005" sheetId="3" r:id="rId3"/>
-    <sheet name="OPR293_DLV_00010" sheetId="4" r:id="rId4"/>
+    <sheet name="OPR293_DLV_00006" sheetId="6" r:id="rId4"/>
+    <sheet name="OPR293_DLV_00010" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="31">
   <si>
     <t>AgentCode</t>
   </si>
@@ -505,28 +506,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5697935-5CF6-4AD9-B921-572906822F3E}">
   <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection sqref="A1:P2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.6328125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.36328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -585,7 +586,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>11377</v>
       </c>
@@ -646,6 +647,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -657,24 +659,24 @@
       <selection activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.6328125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.36328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -733,7 +735,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>11377</v>
       </c>
@@ -802,28 +804,28 @@
   <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.6328125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -885,7 +887,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>11377</v>
       </c>
@@ -953,28 +955,161 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7087D238-E176-4A0F-917B-73F16CD837D3}">
+  <dimension ref="A1:S2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>11377</v>
+      </c>
+      <c r="B2">
+        <v>11377</v>
+      </c>
+      <c r="C2">
+        <v>11377</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2">
+        <v>2</v>
+      </c>
+      <c r="L2">
+        <v>59</v>
+      </c>
+      <c r="M2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N2" t="s">
+        <v>21</v>
+      </c>
+      <c r="O2" t="s">
+        <v>24</v>
+      </c>
+      <c r="P2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>26</v>
+      </c>
+      <c r="R2">
+        <v>2</v>
+      </c>
+      <c r="S2">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C5D376E-C910-4E37-BBE9-957B51BD31E0}">
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.6328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1024,7 +1159,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>11377</v>
       </c>

</xml_diff>